<commit_message>
mcda class structure and correlation implimented
</commit_message>
<xml_diff>
--- a/final_dataset.xlsx
+++ b/final_dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I491"/>
+  <dimension ref="A1:J491"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -479,6 +479,11 @@
           <t>dualclass</t>
         </is>
       </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>mktcapitalisation</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -510,6 +515,9 @@
       <c r="I2" t="n">
         <v>0</v>
       </c>
+      <c r="J2" t="n">
+        <v>39000</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -541,6 +549,9 @@
       <c r="I3" t="n">
         <v>0</v>
       </c>
+      <c r="J3" t="n">
+        <v>8133</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -572,6 +583,9 @@
       <c r="I4" t="n">
         <v>0</v>
       </c>
+      <c r="J4" t="n">
+        <v>2910380</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -603,6 +617,9 @@
       <c r="I5" t="n">
         <v>0</v>
       </c>
+      <c r="J5" t="n">
+        <v>306243</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -634,6 +651,9 @@
       <c r="I6" t="n">
         <v>1</v>
       </c>
+      <c r="J6" t="n">
+        <v>66866</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -665,6 +685,9 @@
       <c r="I7" t="n">
         <v>0</v>
       </c>
+      <c r="J7" t="n">
+        <v>195011</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -696,6 +719,9 @@
       <c r="I8" t="n">
         <v>0</v>
       </c>
+      <c r="J8" t="n">
+        <v>30031</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -727,6 +753,9 @@
       <c r="I9" t="n">
         <v>1</v>
       </c>
+      <c r="J9" t="n">
+        <v>232931</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -758,6 +787,9 @@
       <c r="I10" t="n">
         <v>0</v>
       </c>
+      <c r="J10" t="n">
+        <v>276713</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -789,6 +821,9 @@
       <c r="I11" t="n">
         <v>0</v>
       </c>
+      <c r="J11" t="n">
+        <v>96045</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -820,6 +855,9 @@
       <c r="I12" t="n">
         <v>0</v>
       </c>
+      <c r="J12" t="n">
+        <v>36374</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -851,6 +889,9 @@
       <c r="I13" t="n">
         <v>0</v>
       </c>
+      <c r="J13" t="n">
+        <v>102654</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -882,6 +923,9 @@
       <c r="I14" t="n">
         <v>0</v>
       </c>
+      <c r="J14" t="n">
+        <v>51609</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -913,6 +957,9 @@
       <c r="I15" t="n">
         <v>0</v>
       </c>
+      <c r="J15" t="n">
+        <v>18156</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -944,6 +991,9 @@
       <c r="I16" t="n">
         <v>0</v>
       </c>
+      <c r="J16" t="n">
+        <v>40736</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -975,6 +1025,9 @@
       <c r="I17" t="n">
         <v>0</v>
       </c>
+      <c r="J17" t="n">
+        <v>11642</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1006,6 +1059,9 @@
       <c r="I18" t="n">
         <v>0</v>
       </c>
+      <c r="J18" t="n">
+        <v>45811</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1037,6 +1093,9 @@
       <c r="I19" t="n">
         <v>0</v>
       </c>
+      <c r="J19" t="n">
+        <v>48023</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1068,6 +1127,9 @@
       <c r="I20" t="n">
         <v>0</v>
       </c>
+      <c r="J20" t="n">
+        <v>8762</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1099,6 +1161,9 @@
       <c r="I21" t="n">
         <v>0</v>
       </c>
+      <c r="J21" t="n">
+        <v>50779</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1130,6 +1195,9 @@
       <c r="I22" t="n">
         <v>0</v>
       </c>
+      <c r="J22" t="n">
+        <v>18590</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1161,6 +1229,9 @@
       <c r="I23" t="n">
         <v>0</v>
       </c>
+      <c r="J23" t="n">
+        <v>13275</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1192,6 +1263,9 @@
       <c r="I24" t="n">
         <v>0</v>
       </c>
+      <c r="J24" t="n">
+        <v>19920</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1223,6 +1297,9 @@
       <c r="I25" t="n">
         <v>0</v>
       </c>
+      <c r="J25" t="n">
+        <v>42363</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1254,6 +1331,9 @@
       <c r="I26" t="n">
         <v>0</v>
       </c>
+      <c r="J26" t="n">
+        <v>9312</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1285,6 +1365,9 @@
       <c r="I27" t="n">
         <v>0</v>
       </c>
+      <c r="J27" t="n">
+        <v>154376</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1316,6 +1399,9 @@
       <c r="I28" t="n">
         <v>0</v>
       </c>
+      <c r="J28" t="n">
+        <v>13698</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1347,6 +1433,9 @@
       <c r="I29" t="n">
         <v>0</v>
       </c>
+      <c r="J29" t="n">
+        <v>239926</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1378,6 +1467,9 @@
       <c r="I30" t="n">
         <v>0</v>
       </c>
+      <c r="J30" t="n">
+        <v>38801</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1409,6 +1501,9 @@
       <c r="I31" t="n">
         <v>0</v>
       </c>
+      <c r="J31" t="n">
+        <v>144046</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1440,6 +1535,9 @@
       <c r="I32" t="n">
         <v>0</v>
       </c>
+      <c r="J32" t="n">
+        <v>37930</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1471,6 +1569,9 @@
       <c r="I33" t="n">
         <v>0</v>
       </c>
+      <c r="J33" t="n">
+        <v>91655</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1502,6 +1603,9 @@
       <c r="I34" t="n">
         <v>0</v>
       </c>
+      <c r="J34" t="n">
+        <v>1764193</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1533,6 +1637,9 @@
       <c r="I35" t="n">
         <v>0</v>
       </c>
+      <c r="J35" t="n">
+        <v>83345</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1564,6 +1671,9 @@
       <c r="I36" t="n">
         <v>0</v>
       </c>
+      <c r="J36" t="n">
+        <v>25494</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1595,6 +1705,9 @@
       <c r="I37" t="n">
         <v>0</v>
       </c>
+      <c r="J37" t="n">
+        <v>60024</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1626,6 +1739,9 @@
       <c r="I38" t="n">
         <v>1</v>
       </c>
+      <c r="J38" t="n">
+        <v>9256</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1657,6 +1773,9 @@
       <c r="I39" t="n">
         <v>0</v>
       </c>
+      <c r="J39" t="n">
+        <v>9151</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -1688,6 +1807,9 @@
       <c r="I40" t="n">
         <v>0</v>
       </c>
+      <c r="J40" t="n">
+        <v>47830</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -1719,6 +1841,9 @@
       <c r="I41" t="n">
         <v>0</v>
       </c>
+      <c r="J41" t="n">
+        <v>63029</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -1750,6 +1875,9 @@
       <c r="I42" t="n">
         <v>0</v>
       </c>
+      <c r="J42" t="n">
+        <v>22681</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -1781,6 +1909,9 @@
       <c r="I43" t="n">
         <v>0</v>
       </c>
+      <c r="J43" t="n">
+        <v>17034</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -1812,6 +1943,9 @@
       <c r="I44" t="n">
         <v>0</v>
       </c>
+      <c r="J44" t="n">
+        <v>24690</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -1843,6 +1977,9 @@
       <c r="I45" t="n">
         <v>0</v>
       </c>
+      <c r="J45" t="n">
+        <v>538876</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -1874,6 +2011,9 @@
       <c r="I46" t="n">
         <v>0</v>
       </c>
+      <c r="J46" t="n">
+        <v>16431</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -1905,6 +2045,9 @@
       <c r="I47" t="n">
         <v>0</v>
       </c>
+      <c r="J47" t="n">
+        <v>25672</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -1936,6 +2079,9 @@
       <c r="I48" t="n">
         <v>0</v>
       </c>
+      <c r="J48" t="n">
+        <v>17233</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -1967,6 +2113,9 @@
       <c r="I49" t="n">
         <v>0</v>
       </c>
+      <c r="J49" t="n">
+        <v>151897</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -1998,6 +2147,9 @@
       <c r="I50" t="n">
         <v>0</v>
       </c>
+      <c r="J50" t="n">
+        <v>44647</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2029,6 +2181,9 @@
       <c r="I51" t="n">
         <v>0</v>
       </c>
+      <c r="J51" t="n">
+        <v>130843</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2060,6 +2215,9 @@
       <c r="I52" t="n">
         <v>0</v>
       </c>
+      <c r="J52" t="n">
+        <v>258599</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2091,6 +2249,9 @@
       <c r="I53" t="n">
         <v>0</v>
       </c>
+      <c r="J53" t="n">
+        <v>17599</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2122,6 +2283,9 @@
       <c r="I54" t="n">
         <v>0</v>
       </c>
+      <c r="J54" t="n">
+        <v>20421</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2153,6 +2317,9 @@
       <c r="I55" t="n">
         <v>0</v>
       </c>
+      <c r="J55" t="n">
+        <v>7960</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2184,6 +2351,9 @@
       <c r="I56" t="n">
         <v>0</v>
       </c>
+      <c r="J56" t="n">
+        <v>15275</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2215,6 +2385,9 @@
       <c r="I57" t="n">
         <v>0</v>
       </c>
+      <c r="J57" t="n">
+        <v>68331</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2246,6 +2419,9 @@
       <c r="I58" t="n">
         <v>0</v>
       </c>
+      <c r="J58" t="n">
+        <v>14120</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2277,6 +2453,9 @@
       <c r="I59" t="n">
         <v>1</v>
       </c>
+      <c r="J59" t="n">
+        <v>26870</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2308,6 +2487,9 @@
       <c r="I60" t="n">
         <v>0</v>
       </c>
+      <c r="J60" t="n">
+        <v>13097</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2339,6 +2521,9 @@
       <c r="I61" t="n">
         <v>0</v>
       </c>
+      <c r="J61" t="n">
+        <v>37361</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2370,6 +2555,9 @@
       <c r="I62" t="n">
         <v>1</v>
       </c>
+      <c r="J62" t="n">
+        <v>8887</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2401,6 +2589,9 @@
       <c r="I63" t="n">
         <v>0</v>
       </c>
+      <c r="J63" t="n">
+        <v>39976</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2432,6 +2623,9 @@
       <c r="I64" t="n">
         <v>0</v>
       </c>
+      <c r="J64" t="n">
+        <v>111494</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -2463,6 +2657,9 @@
       <c r="I65" t="n">
         <v>1</v>
       </c>
+      <c r="J65" t="n">
+        <v>29256</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -2494,6 +2691,9 @@
       <c r="I66" t="n">
         <v>0</v>
       </c>
+      <c r="J66" t="n">
+        <v>20688</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -2525,6 +2725,9 @@
       <c r="I67" t="n">
         <v>0</v>
       </c>
+      <c r="J67" t="n">
+        <v>119092</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -2556,6 +2759,9 @@
       <c r="I68" t="n">
         <v>0</v>
       </c>
+      <c r="J68" t="n">
+        <v>100609</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -2587,6 +2793,9 @@
       <c r="I69" t="n">
         <v>0</v>
       </c>
+      <c r="J69" t="n">
+        <v>23485</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -2618,6 +2827,9 @@
       <c r="I70" t="n">
         <v>1</v>
       </c>
+      <c r="J70" t="n">
+        <v>785207</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -2649,6 +2861,9 @@
       <c r="I71" t="n">
         <v>0</v>
       </c>
+      <c r="J71" t="n">
+        <v>23010</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -2680,6 +2895,9 @@
       <c r="I72" t="n">
         <v>0</v>
       </c>
+      <c r="J72" t="n">
+        <v>81885</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -2711,6 +2929,9 @@
       <c r="I73" t="n">
         <v>0</v>
       </c>
+      <c r="J73" t="n">
+        <v>7412</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -2742,6 +2963,9 @@
       <c r="I74" t="n">
         <v>0</v>
       </c>
+      <c r="J74" t="n">
+        <v>8934</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -2773,6 +2997,9 @@
       <c r="I75" t="n">
         <v>0</v>
       </c>
+      <c r="J75" t="n">
+        <v>98662</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -2804,6 +3031,9 @@
       <c r="I76" t="n">
         <v>0</v>
       </c>
+      <c r="J76" t="n">
+        <v>13931</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -2835,6 +3065,9 @@
       <c r="I77" t="n">
         <v>0</v>
       </c>
+      <c r="J77" t="n">
+        <v>25991</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -2866,6 +3099,9 @@
       <c r="I78" t="n">
         <v>0</v>
       </c>
+      <c r="J78" t="n">
+        <v>45818</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -2897,6 +3133,9 @@
       <c r="I79" t="n">
         <v>0</v>
       </c>
+      <c r="J79" t="n">
+        <v>127911</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -2928,6 +3167,9 @@
       <c r="I80" t="n">
         <v>0</v>
       </c>
+      <c r="J80" t="n">
+        <v>100523</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -2959,6 +3201,9 @@
       <c r="I81" t="n">
         <v>0</v>
       </c>
+      <c r="J81" t="n">
+        <v>19646</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -2990,6 +3235,9 @@
       <c r="I82" t="n">
         <v>0</v>
       </c>
+      <c r="J82" t="n">
+        <v>25683</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3021,6 +3269,9 @@
       <c r="I83" t="n">
         <v>0</v>
       </c>
+      <c r="J83" t="n">
+        <v>47402</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3052,6 +3303,9 @@
       <c r="I84" t="n">
         <v>0</v>
       </c>
+      <c r="J84" t="n">
+        <v>17559</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3083,6 +3337,9 @@
       <c r="I85" t="n">
         <v>0</v>
       </c>
+      <c r="J85" t="n">
+        <v>81205</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3114,6 +3371,9 @@
       <c r="I86" t="n">
         <v>0</v>
       </c>
+      <c r="J86" t="n">
+        <v>28265</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3145,6 +3405,9 @@
       <c r="I87" t="n">
         <v>0</v>
       </c>
+      <c r="J87" t="n">
+        <v>16180</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3176,6 +3439,9 @@
       <c r="I88" t="n">
         <v>0</v>
       </c>
+      <c r="J88" t="n">
+        <v>38653</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3207,6 +3473,9 @@
       <c r="I89" t="n">
         <v>0</v>
       </c>
+      <c r="J89" t="n">
+        <v>14633</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -3238,6 +3507,9 @@
       <c r="I90" t="n">
         <v>0</v>
       </c>
+      <c r="J90" t="n">
+        <v>14796</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -3269,6 +3541,9 @@
       <c r="I91" t="n">
         <v>0</v>
       </c>
+      <c r="J91" t="n">
+        <v>23787</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -3300,6 +3575,9 @@
       <c r="I92" t="n">
         <v>0</v>
       </c>
+      <c r="J92" t="n">
+        <v>9854</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -3331,6 +3609,9 @@
       <c r="I93" t="n">
         <v>0</v>
       </c>
+      <c r="J93" t="n">
+        <v>43189</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -3362,6 +3643,9 @@
       <c r="I94" t="n">
         <v>0</v>
       </c>
+      <c r="J94" t="n">
+        <v>97778</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -3393,6 +3677,9 @@
       <c r="I95" t="n">
         <v>0</v>
       </c>
+      <c r="J95" t="n">
+        <v>17590</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -3424,6 +3711,9 @@
       <c r="I96" t="n">
         <v>0</v>
       </c>
+      <c r="J96" t="n">
+        <v>65131</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -3455,6 +3745,9 @@
       <c r="I97" t="n">
         <v>0</v>
       </c>
+      <c r="J97" t="n">
+        <v>17573</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -3486,6 +3779,9 @@
       <c r="I98" t="n">
         <v>0</v>
       </c>
+      <c r="J98" t="n">
+        <v>6776</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -3517,6 +3813,9 @@
       <c r="I99" t="n">
         <v>1</v>
       </c>
+      <c r="J99" t="n">
+        <v>165609</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -3548,6 +3847,9 @@
       <c r="I100" t="n">
         <v>1</v>
       </c>
+      <c r="J100" t="n">
+        <v>77365</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -3579,6 +3881,9 @@
       <c r="I101" t="n">
         <v>0</v>
       </c>
+      <c r="J101" t="n">
+        <v>71435</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -3610,6 +3915,9 @@
       <c r="I102" t="n">
         <v>0</v>
       </c>
+      <c r="J102" t="n">
+        <v>37053</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -3641,6 +3949,9 @@
       <c r="I103" t="n">
         <v>0</v>
       </c>
+      <c r="J103" t="n">
+        <v>16742</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -3672,6 +3983,9 @@
       <c r="I104" t="n">
         <v>0</v>
       </c>
+      <c r="J104" t="n">
+        <v>39620</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -3703,6 +4017,9 @@
       <c r="I105" t="n">
         <v>0</v>
       </c>
+      <c r="J105" t="n">
+        <v>18359</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -3734,6 +4051,9 @@
       <c r="I106" t="n">
         <v>0</v>
       </c>
+      <c r="J106" t="n">
+        <v>49162</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -3765,6 +4085,9 @@
       <c r="I107" t="n">
         <v>0</v>
       </c>
+      <c r="J107" t="n">
+        <v>18281</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -3796,6 +4119,9 @@
       <c r="I108" t="n">
         <v>0</v>
       </c>
+      <c r="J108" t="n">
+        <v>138364</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -3827,6 +4153,9 @@
       <c r="I109" t="n">
         <v>0</v>
       </c>
+      <c r="J109" t="n">
+        <v>45814</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -3858,6 +4187,9 @@
       <c r="I110" t="n">
         <v>0</v>
       </c>
+      <c r="J110" t="n">
+        <v>320278</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -3889,6 +4221,9 @@
       <c r="I111" t="n">
         <v>0</v>
       </c>
+      <c r="J111" t="n">
+        <v>13062</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -3920,6 +4255,9 @@
       <c r="I112" t="n">
         <v>0</v>
       </c>
+      <c r="J112" t="n">
+        <v>45620</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -3951,6 +4289,9 @@
       <c r="I113" t="n">
         <v>0</v>
       </c>
+      <c r="J113" t="n">
+        <v>9639</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -3982,6 +4323,9 @@
       <c r="I114" t="n">
         <v>0</v>
       </c>
+      <c r="J114" t="n">
+        <v>10921</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -4013,6 +4357,9 @@
       <c r="I115" t="n">
         <v>0</v>
       </c>
+      <c r="J115" t="n">
+        <v>282588</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -4044,6 +4391,9 @@
       <c r="I116" t="n">
         <v>0</v>
       </c>
+      <c r="J116" t="n">
+        <v>202158</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -4075,6 +4425,9 @@
       <c r="I117" t="n">
         <v>0</v>
       </c>
+      <c r="J117" t="n">
+        <v>33768</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -4106,6 +4459,9 @@
       <c r="I118" t="n">
         <v>0</v>
       </c>
+      <c r="J118" t="n">
+        <v>63839</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -4137,6 +4493,9 @@
       <c r="I119" t="n">
         <v>0</v>
       </c>
+      <c r="J119" t="n">
+        <v>60794</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -4168,6 +4527,9 @@
       <c r="I120" t="n">
         <v>0</v>
       </c>
+      <c r="J120" t="n">
+        <v>19741</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -4199,6 +4561,9 @@
       <c r="I121" t="n">
         <v>0</v>
       </c>
+      <c r="J121" t="n">
+        <v>38317</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -4230,6 +4595,9 @@
       <c r="I122" t="n">
         <v>0</v>
       </c>
+      <c r="J122" t="n">
+        <v>38563</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -4261,6 +4629,9 @@
       <c r="I123" t="n">
         <v>0</v>
       </c>
+      <c r="J123" t="n">
+        <v>87204</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -4292,6 +4663,9 @@
       <c r="I124" t="n">
         <v>0</v>
       </c>
+      <c r="J124" t="n">
+        <v>287060</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -4323,6 +4697,9 @@
       <c r="I125" t="n">
         <v>0</v>
       </c>
+      <c r="J125" t="n">
+        <v>9648</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -4354,6 +4731,9 @@
       <c r="I126" t="n">
         <v>0</v>
       </c>
+      <c r="J126" t="n">
+        <v>37773</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -4385,6 +4765,9 @@
       <c r="I127" t="n">
         <v>0</v>
       </c>
+      <c r="J127" t="n">
+        <v>26074</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -4416,6 +4799,9 @@
       <c r="I128" t="n">
         <v>0</v>
       </c>
+      <c r="J128" t="n">
+        <v>31535</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -4447,6 +4833,9 @@
       <c r="I129" t="n">
         <v>0</v>
       </c>
+      <c r="J129" t="n">
+        <v>107840</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -4478,6 +4867,9 @@
       <c r="I130" t="n">
         <v>0</v>
       </c>
+      <c r="J130" t="n">
+        <v>26387</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -4509,6 +4901,9 @@
       <c r="I131" t="n">
         <v>0</v>
       </c>
+      <c r="J131" t="n">
+        <v>29844</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -4540,6 +4935,9 @@
       <c r="I132" t="n">
         <v>0</v>
       </c>
+      <c r="J132" t="n">
+        <v>15476</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -4571,6 +4969,9 @@
       <c r="I133" t="n">
         <v>0</v>
       </c>
+      <c r="J133" t="n">
+        <v>178705</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -4602,6 +5003,9 @@
       <c r="I134" t="n">
         <v>0</v>
       </c>
+      <c r="J134" t="n">
+        <v>198357</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -4633,6 +5037,9 @@
       <c r="I135" t="n">
         <v>0</v>
       </c>
+      <c r="J135" t="n">
+        <v>41159</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -4664,6 +5071,9 @@
       <c r="I136" t="n">
         <v>0</v>
       </c>
+      <c r="J136" t="n">
+        <v>27216</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -4695,6 +5105,9 @@
       <c r="I137" t="n">
         <v>0</v>
       </c>
+      <c r="J137" t="n">
+        <v>22570</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -4726,6 +5139,9 @@
       <c r="I138" t="n">
         <v>0</v>
       </c>
+      <c r="J138" t="n">
+        <v>37836</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -4757,6 +5173,9 @@
       <c r="I139" t="n">
         <v>0</v>
       </c>
+      <c r="J139" t="n">
+        <v>13711</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -4788,6 +5207,9 @@
       <c r="I140" t="n">
         <v>0</v>
       </c>
+      <c r="J140" t="n">
+        <v>18878</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -4819,6 +5241,9 @@
       <c r="I141" t="n">
         <v>0</v>
       </c>
+      <c r="J141" t="n">
+        <v>22047</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -4850,6 +5275,9 @@
       <c r="I142" t="n">
         <v>0</v>
       </c>
+      <c r="J142" t="n">
+        <v>70685</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -4881,6 +5309,9 @@
       <c r="I143" t="n">
         <v>0</v>
       </c>
+      <c r="J143" t="n">
+        <v>9258</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -4912,6 +5343,9 @@
       <c r="I144" t="n">
         <v>0</v>
       </c>
+      <c r="J144" t="n">
+        <v>28803</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -4943,6 +5377,9 @@
       <c r="I145" t="n">
         <v>0</v>
       </c>
+      <c r="J145" t="n">
+        <v>45431</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -4974,6 +5411,9 @@
       <c r="I146" t="n">
         <v>0</v>
       </c>
+      <c r="J146" t="n">
+        <v>37122</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -5005,6 +5445,9 @@
       <c r="I147" t="n">
         <v>0</v>
       </c>
+      <c r="J147" t="n">
+        <v>22128</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -5036,6 +5479,9 @@
       <c r="I148" t="n">
         <v>0</v>
       </c>
+      <c r="J148" t="n">
+        <v>57143</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -5067,6 +5513,9 @@
       <c r="I149" t="n">
         <v>0</v>
       </c>
+      <c r="J149" t="n">
+        <v>31531</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -5098,6 +5547,9 @@
       <c r="I150" t="n">
         <v>0</v>
       </c>
+      <c r="J150" t="n">
+        <v>30224</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -5129,6 +5581,9 @@
       <c r="I151" t="n">
         <v>0</v>
       </c>
+      <c r="J151" t="n">
+        <v>15882</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -5160,6 +5615,9 @@
       <c r="I152" t="n">
         <v>0</v>
       </c>
+      <c r="J152" t="n">
+        <v>24769</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -5191,6 +5649,9 @@
       <c r="I153" t="n">
         <v>1</v>
       </c>
+      <c r="J153" t="n">
+        <v>33926</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -5222,6 +5683,9 @@
       <c r="I154" t="n">
         <v>0</v>
       </c>
+      <c r="J154" t="n">
+        <v>118680</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -5253,6 +5717,9 @@
       <c r="I155" t="n">
         <v>0</v>
       </c>
+      <c r="J155" t="n">
+        <v>9937</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -5284,6 +5751,9 @@
       <c r="I156" t="n">
         <v>0</v>
       </c>
+      <c r="J156" t="n">
+        <v>58878</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -5315,6 +5785,9 @@
       <c r="I157" t="n">
         <v>0</v>
       </c>
+      <c r="J157" t="n">
+        <v>16792</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -5346,6 +5819,9 @@
       <c r="I158" t="n">
         <v>0</v>
       </c>
+      <c r="J158" t="n">
+        <v>70255</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -5377,6 +5853,9 @@
       <c r="I159" t="n">
         <v>0</v>
       </c>
+      <c r="J159" t="n">
+        <v>16734</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -5408,6 +5887,9 @@
       <c r="I160" t="n">
         <v>0</v>
       </c>
+      <c r="J160" t="n">
+        <v>75183</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -5439,6 +5921,9 @@
       <c r="I161" t="n">
         <v>0</v>
       </c>
+      <c r="J161" t="n">
+        <v>21582</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -5470,6 +5955,9 @@
       <c r="I162" t="n">
         <v>0</v>
       </c>
+      <c r="J162" t="n">
+        <v>14348</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -5501,6 +5989,9 @@
       <c r="I163" t="n">
         <v>0</v>
       </c>
+      <c r="J163" t="n">
+        <v>21772</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -5532,6 +6023,9 @@
       <c r="I164" t="n">
         <v>0</v>
       </c>
+      <c r="J164" t="n">
+        <v>15855</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -5563,6 +6057,9 @@
       <c r="I165" t="n">
         <v>0</v>
       </c>
+      <c r="J165" t="n">
+        <v>107694</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -5594,6 +6091,9 @@
       <c r="I166" t="n">
         <v>0</v>
       </c>
+      <c r="J166" t="n">
+        <v>21897</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -5625,6 +6125,9 @@
       <c r="I167" t="n">
         <v>0</v>
       </c>
+      <c r="J167" t="n">
+        <v>9051</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -5656,6 +6159,9 @@
       <c r="I168" t="n">
         <v>0</v>
       </c>
+      <c r="J168" t="n">
+        <v>11649</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -5687,6 +6193,9 @@
       <c r="I169" t="n">
         <v>0</v>
       </c>
+      <c r="J169" t="n">
+        <v>41066</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -5718,6 +6227,9 @@
       <c r="I170" t="n">
         <v>0</v>
       </c>
+      <c r="J170" t="n">
+        <v>33794</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -5749,6 +6261,9 @@
       <c r="I171" t="n">
         <v>0</v>
       </c>
+      <c r="J171" t="n">
+        <v>18366</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -5780,6 +6295,9 @@
       <c r="I172" t="n">
         <v>1</v>
       </c>
+      <c r="J172" t="n">
+        <v>21313</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -5811,6 +6329,9 @@
       <c r="I173" t="n">
         <v>0</v>
       </c>
+      <c r="J173" t="n">
+        <v>27513</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -5842,6 +6363,9 @@
       <c r="I174" t="n">
         <v>1</v>
       </c>
+      <c r="J174" t="n">
+        <v>48843</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -5873,6 +6397,9 @@
       <c r="I175" t="n">
         <v>0</v>
       </c>
+      <c r="J175" t="n">
+        <v>27631</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -5904,6 +6431,9 @@
       <c r="I176" t="n">
         <v>0</v>
       </c>
+      <c r="J176" t="n">
+        <v>39624</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -5935,6 +6465,9 @@
       <c r="I177" t="n">
         <v>0</v>
       </c>
+      <c r="J177" t="n">
+        <v>57668</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -5966,6 +6499,9 @@
       <c r="I178" t="n">
         <v>0</v>
       </c>
+      <c r="J178" t="n">
+        <v>17402</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -5997,6 +6533,9 @@
       <c r="I179" t="n">
         <v>0</v>
       </c>
+      <c r="J179" t="n">
+        <v>60591</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -6028,6 +6567,9 @@
       <c r="I180" t="n">
         <v>0</v>
       </c>
+      <c r="J180" t="n">
+        <v>21424</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -6059,6 +6601,9 @@
       <c r="I181" t="n">
         <v>0</v>
       </c>
+      <c r="J181" t="n">
+        <v>10794</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -6090,6 +6635,9 @@
       <c r="I182" t="n">
         <v>0</v>
       </c>
+      <c r="J182" t="n">
+        <v>88830</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -6121,6 +6669,9 @@
       <c r="I183" t="n">
         <v>0</v>
       </c>
+      <c r="J183" t="n">
+        <v>29926</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -6152,6 +6703,9 @@
       <c r="I184" t="n">
         <v>0</v>
       </c>
+      <c r="J184" t="n">
+        <v>37227</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -6183,6 +6737,9 @@
       <c r="I185" t="n">
         <v>0</v>
       </c>
+      <c r="J185" t="n">
+        <v>23793</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -6214,6 +6771,9 @@
       <c r="I186" t="n">
         <v>0</v>
       </c>
+      <c r="J186" t="n">
+        <v>19523</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -6245,6 +6805,9 @@
       <c r="I187" t="n">
         <v>0</v>
       </c>
+      <c r="J187" t="n">
+        <v>7834</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -6276,6 +6839,9 @@
       <c r="I188" t="n">
         <v>1</v>
       </c>
+      <c r="J188" t="n">
+        <v>14647</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -6307,6 +6873,9 @@
       <c r="I189" t="n">
         <v>0</v>
       </c>
+      <c r="J189" t="n">
+        <v>8397</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -6338,6 +6907,9 @@
       <c r="I190" t="n">
         <v>0</v>
       </c>
+      <c r="J190" t="n">
+        <v>17345</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -6369,6 +6941,9 @@
       <c r="I191" t="n">
         <v>0</v>
       </c>
+      <c r="J191" t="n">
+        <v>50730</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -6400,6 +6975,9 @@
       <c r="I192" t="n">
         <v>0</v>
       </c>
+      <c r="J192" t="n">
+        <v>24978</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -6431,6 +7009,9 @@
       <c r="I193" t="n">
         <v>0</v>
       </c>
+      <c r="J193" t="n">
+        <v>73938</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -6462,6 +7043,9 @@
       <c r="I194" t="n">
         <v>0</v>
       </c>
+      <c r="J194" t="n">
+        <v>159897</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -6493,6 +7077,9 @@
       <c r="I195" t="n">
         <v>0</v>
       </c>
+      <c r="J195" t="n">
+        <v>38999</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -6524,6 +7111,9 @@
       <c r="I196" t="n">
         <v>0</v>
       </c>
+      <c r="J196" t="n">
+        <v>13635</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -6555,6 +7145,9 @@
       <c r="I197" t="n">
         <v>0</v>
       </c>
+      <c r="J197" t="n">
+        <v>95744</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -6586,6 +7179,9 @@
       <c r="I198" t="n">
         <v>0</v>
       </c>
+      <c r="J198" t="n">
+        <v>95744</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -6617,6 +7213,9 @@
       <c r="I199" t="n">
         <v>0</v>
       </c>
+      <c r="J199" t="n">
+        <v>11501</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -6648,6 +7247,9 @@
       <c r="I200" t="n">
         <v>0</v>
       </c>
+      <c r="J200" t="n">
+        <v>27183</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -6679,6 +7281,9 @@
       <c r="I201" t="n">
         <v>0</v>
       </c>
+      <c r="J201" t="n">
+        <v>44625</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -6710,6 +7315,9 @@
       <c r="I202" t="n">
         <v>0</v>
       </c>
+      <c r="J202" t="n">
+        <v>7288</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -6741,6 +7349,9 @@
       <c r="I203" t="n">
         <v>1</v>
       </c>
+      <c r="J203" t="n">
+        <v>1682489</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -6772,6 +7383,9 @@
       <c r="I204" t="n">
         <v>0</v>
       </c>
+      <c r="J204" t="n">
+        <v>20313</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -6803,6 +7417,9 @@
       <c r="I205" t="n">
         <v>0</v>
       </c>
+      <c r="J205" t="n">
+        <v>32942</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -6834,6 +7451,9 @@
       <c r="I206" t="n">
         <v>0</v>
       </c>
+      <c r="J206" t="n">
+        <v>23389</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -6865,6 +7485,9 @@
       <c r="I207" t="n">
         <v>0</v>
       </c>
+      <c r="J207" t="n">
+        <v>123674</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -6896,6 +7519,9 @@
       <c r="I208" t="n">
         <v>0</v>
       </c>
+      <c r="J208" t="n">
+        <v>46961</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -6927,6 +7553,9 @@
       <c r="I209" t="n">
         <v>0</v>
       </c>
+      <c r="J209" t="n">
+        <v>31452</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -6958,6 +7587,9 @@
       <c r="I210" t="n">
         <v>0</v>
       </c>
+      <c r="J210" t="n">
+        <v>6440</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -6989,6 +7621,9 @@
       <c r="I211" t="n">
         <v>0</v>
       </c>
+      <c r="J211" t="n">
+        <v>16313</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -7020,6 +7655,9 @@
       <c r="I212" t="n">
         <v>0</v>
       </c>
+      <c r="J212" t="n">
+        <v>82818</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -7051,6 +7689,9 @@
       <c r="I213" t="n">
         <v>0</v>
       </c>
+      <c r="J213" t="n">
+        <v>346223</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -7082,6 +7723,9 @@
       <c r="I214" t="n">
         <v>0</v>
       </c>
+      <c r="J214" t="n">
+        <v>43145</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -7113,6 +7757,9 @@
       <c r="I215" t="n">
         <v>0</v>
       </c>
+      <c r="J215" t="n">
+        <v>23504</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -7144,6 +7791,9 @@
       <c r="I216" t="n">
         <v>0</v>
       </c>
+      <c r="J216" t="n">
+        <v>10896</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -7175,6 +7825,9 @@
       <c r="I217" t="n">
         <v>0</v>
       </c>
+      <c r="J217" t="n">
+        <v>49475</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -7206,6 +7859,9 @@
       <c r="I218" t="n">
         <v>0</v>
       </c>
+      <c r="J218" t="n">
+        <v>17354</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -7237,6 +7893,9 @@
       <c r="I219" t="n">
         <v>0</v>
       </c>
+      <c r="J219" t="n">
+        <v>128186</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -7268,6 +7927,9 @@
       <c r="I220" t="n">
         <v>0</v>
       </c>
+      <c r="J220" t="n">
+        <v>19743</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -7299,6 +7961,9 @@
       <c r="I221" t="n">
         <v>0</v>
       </c>
+      <c r="J221" t="n">
+        <v>28782</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -7330,6 +7995,9 @@
       <c r="I222" t="n">
         <v>0</v>
       </c>
+      <c r="J222" t="n">
+        <v>16399</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -7361,6 +8029,9 @@
       <c r="I223" t="n">
         <v>0</v>
       </c>
+      <c r="J223" t="n">
+        <v>9695</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -7392,6 +8063,9 @@
       <c r="I224" t="n">
         <v>0</v>
       </c>
+      <c r="J224" t="n">
+        <v>12328</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -7423,6 +8097,9 @@
       <c r="I225" t="n">
         <v>1</v>
       </c>
+      <c r="J225" t="n">
+        <v>28985</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -7454,6 +8131,9 @@
       <c r="I226" t="n">
         <v>0</v>
       </c>
+      <c r="J226" t="n">
+        <v>18933</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -7485,6 +8165,9 @@
       <c r="I227" t="n">
         <v>0</v>
       </c>
+      <c r="J227" t="n">
+        <v>46594</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -7516,6 +8199,9 @@
       <c r="I228" t="n">
         <v>0</v>
       </c>
+      <c r="J228" t="n">
+        <v>25962</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -7547,6 +8233,9 @@
       <c r="I229" t="n">
         <v>0</v>
       </c>
+      <c r="J229" t="n">
+        <v>169708</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -7578,6 +8267,9 @@
       <c r="I230" t="n">
         <v>0</v>
       </c>
+      <c r="J230" t="n">
+        <v>73228</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -7609,6 +8301,9 @@
       <c r="I231" t="n">
         <v>0</v>
       </c>
+      <c r="J231" t="n">
+        <v>44207</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -7640,6 +8335,9 @@
       <c r="I232" t="n">
         <v>0</v>
       </c>
+      <c r="J232" t="n">
+        <v>15544</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -7671,6 +8369,9 @@
       <c r="I233" t="n">
         <v>0</v>
       </c>
+      <c r="J233" t="n">
+        <v>20600</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -7702,6 +8403,9 @@
       <c r="I234" t="n">
         <v>0</v>
       </c>
+      <c r="J234" t="n">
+        <v>22381</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -7733,6 +8437,9 @@
       <c r="I235" t="n">
         <v>0</v>
       </c>
+      <c r="J235" t="n">
+        <v>12179</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -7764,6 +8471,9 @@
       <c r="I236" t="n">
         <v>0</v>
       </c>
+      <c r="J236" t="n">
+        <v>185841</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -7795,6 +8505,9 @@
       <c r="I237" t="n">
         <v>0</v>
       </c>
+      <c r="J237" t="n">
+        <v>174274</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -7826,6 +8539,9 @@
       <c r="I238" t="n">
         <v>0</v>
       </c>
+      <c r="J238" t="n">
+        <v>20409</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -7857,6 +8573,9 @@
       <c r="I239" t="n">
         <v>0</v>
       </c>
+      <c r="J239" t="n">
+        <v>12791</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -7888,6 +8607,9 @@
       <c r="I240" t="n">
         <v>0</v>
       </c>
+      <c r="J240" t="n">
+        <v>12181</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -7919,6 +8641,9 @@
       <c r="I241" t="n">
         <v>0</v>
       </c>
+      <c r="J241" t="n">
+        <v>44567</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -7950,6 +8675,9 @@
       <c r="I242" t="n">
         <v>0</v>
       </c>
+      <c r="J242" t="n">
+        <v>61992</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -7981,6 +8709,9 @@
       <c r="I243" t="n">
         <v>0</v>
       </c>
+      <c r="J243" t="n">
+        <v>18727</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -8012,6 +8743,9 @@
       <c r="I244" t="n">
         <v>0</v>
       </c>
+      <c r="J244" t="n">
+        <v>109311</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -8043,6 +8777,9 @@
       <c r="I245" t="n">
         <v>0</v>
       </c>
+      <c r="J245" t="n">
+        <v>35155</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -8074,6 +8811,9 @@
       <c r="I246" t="n">
         <v>0</v>
       </c>
+      <c r="J246" t="n">
+        <v>75293</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -8105,6 +8845,9 @@
       <c r="I247" t="n">
         <v>0</v>
       </c>
+      <c r="J247" t="n">
+        <v>6740</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -8136,6 +8879,9 @@
       <c r="I248" t="n">
         <v>0</v>
       </c>
+      <c r="J248" t="n">
+        <v>17986</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -8167,6 +8913,9 @@
       <c r="I249" t="n">
         <v>0</v>
       </c>
+      <c r="J249" t="n">
+        <v>19810</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -8198,6 +8947,9 @@
       <c r="I250" t="n">
         <v>0</v>
       </c>
+      <c r="J250" t="n">
+        <v>17700</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -8229,6 +8981,9 @@
       <c r="I251" t="n">
         <v>0</v>
       </c>
+      <c r="J251" t="n">
+        <v>37560</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -8260,6 +9015,9 @@
       <c r="I252" t="n">
         <v>0</v>
       </c>
+      <c r="J252" t="n">
+        <v>12774</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -8291,6 +9049,9 @@
       <c r="I253" t="n">
         <v>0</v>
       </c>
+      <c r="J253" t="n">
+        <v>379357</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -8322,6 +9083,9 @@
       <c r="I254" t="n">
         <v>0</v>
       </c>
+      <c r="J254" t="n">
+        <v>11896</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -8353,6 +9117,9 @@
       <c r="I255" t="n">
         <v>0</v>
       </c>
+      <c r="J255" t="n">
+        <v>504033</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -8384,6 +9151,9 @@
       <c r="I256" t="n">
         <v>0</v>
       </c>
+      <c r="J256" t="n">
+        <v>18690</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -8415,6 +9185,9 @@
       <c r="I257" t="n">
         <v>0</v>
       </c>
+      <c r="J257" t="n">
+        <v>44555</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -8446,6 +9219,9 @@
       <c r="I258" t="n">
         <v>0</v>
       </c>
+      <c r="J258" t="n">
+        <v>13963</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -8477,6 +9253,9 @@
       <c r="I259" t="n">
         <v>0</v>
       </c>
+      <c r="J259" t="n">
+        <v>27133</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -8508,6 +9287,9 @@
       <c r="I260" t="n">
         <v>0</v>
       </c>
+      <c r="J260" t="n">
+        <v>45190</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -8539,6 +9321,9 @@
       <c r="I261" t="n">
         <v>0</v>
       </c>
+      <c r="J261" t="n">
+        <v>14031</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -8570,6 +9355,9 @@
       <c r="I262" t="n">
         <v>0</v>
       </c>
+      <c r="J262" t="n">
+        <v>81608</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -8601,6 +9389,9 @@
       <c r="I263" t="n">
         <v>0</v>
       </c>
+      <c r="J263" t="n">
+        <v>40374</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -8632,6 +9423,9 @@
       <c r="I264" t="n">
         <v>0</v>
       </c>
+      <c r="J264" t="n">
+        <v>39109</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -8663,6 +9457,9 @@
       <c r="I265" t="n">
         <v>0</v>
       </c>
+      <c r="J265" t="n">
+        <v>10137</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -8694,6 +9491,9 @@
       <c r="I266" t="n">
         <v>0</v>
       </c>
+      <c r="J266" t="n">
+        <v>258389</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -8725,6 +9525,9 @@
       <c r="I267" t="n">
         <v>0</v>
       </c>
+      <c r="J267" t="n">
+        <v>32933</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -8756,6 +9559,9 @@
       <c r="I268" t="n">
         <v>0</v>
       </c>
+      <c r="J268" t="n">
+        <v>30350</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -8787,6 +9593,9 @@
       <c r="I269" t="n">
         <v>0</v>
       </c>
+      <c r="J269" t="n">
+        <v>16586</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -8818,6 +9627,9 @@
       <c r="I270" t="n">
         <v>1</v>
       </c>
+      <c r="J270" t="n">
+        <v>43905</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -8849,6 +9661,9 @@
       <c r="I271" t="n">
         <v>0</v>
       </c>
+      <c r="J271" t="n">
+        <v>18410</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -8880,6 +9695,9 @@
       <c r="I272" t="n">
         <v>0</v>
       </c>
+      <c r="J272" t="n">
+        <v>37782</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -8911,6 +9729,9 @@
       <c r="I273" t="n">
         <v>0</v>
       </c>
+      <c r="J273" t="n">
+        <v>201917</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -8942,6 +9763,9 @@
       <c r="I274" t="n">
         <v>0</v>
       </c>
+      <c r="J274" t="n">
+        <v>12661</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -8973,6 +9797,9 @@
       <c r="I275" t="n">
         <v>0</v>
       </c>
+      <c r="J275" t="n">
+        <v>669551</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -9004,6 +9831,9 @@
       <c r="I276" t="n">
         <v>0</v>
       </c>
+      <c r="J276" t="n">
+        <v>101290</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -9035,6 +9865,9 @@
       <c r="I277" t="n">
         <v>0</v>
       </c>
+      <c r="J277" t="n">
+        <v>13040</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -9066,6 +9899,9 @@
       <c r="I278" t="n">
         <v>0</v>
       </c>
+      <c r="J278" t="n">
+        <v>125431</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -9097,6 +9933,9 @@
       <c r="I279" t="n">
         <v>0</v>
       </c>
+      <c r="J279" t="n">
+        <v>94425</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -9128,6 +9967,9 @@
       <c r="I280" t="n">
         <v>0</v>
       </c>
+      <c r="J280" t="n">
+        <v>57806</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -9159,6 +10001,9 @@
       <c r="I281" t="n">
         <v>0</v>
       </c>
+      <c r="J281" t="n">
+        <v>19287</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -9190,6 +10035,9 @@
       <c r="I282" t="n">
         <v>0</v>
       </c>
+      <c r="J282" t="n">
+        <v>40975</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -9221,6 +10069,9 @@
       <c r="I283" t="n">
         <v>0</v>
       </c>
+      <c r="J283" t="n">
+        <v>15536</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -9252,6 +10103,9 @@
       <c r="I284" t="n">
         <v>0</v>
       </c>
+      <c r="J284" t="n">
+        <v>30636</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -9283,6 +10137,9 @@
       <c r="I285" t="n">
         <v>0</v>
       </c>
+      <c r="J285" t="n">
+        <v>21555</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -9314,6 +10171,9 @@
       <c r="I286" t="n">
         <v>1</v>
       </c>
+      <c r="J286" t="n">
+        <v>404856</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -9345,6 +10205,9 @@
       <c r="I287" t="n">
         <v>0</v>
       </c>
+      <c r="J287" t="n">
+        <v>14408</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -9376,6 +10239,9 @@
       <c r="I288" t="n">
         <v>0</v>
       </c>
+      <c r="J288" t="n">
+        <v>60455</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -9407,6 +10273,9 @@
       <c r="I289" t="n">
         <v>0</v>
       </c>
+      <c r="J289" t="n">
+        <v>16074</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -9438,6 +10307,9 @@
       <c r="I290" t="n">
         <v>0</v>
       </c>
+      <c r="J290" t="n">
+        <v>205384</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -9469,6 +10341,9 @@
       <c r="I291" t="n">
         <v>0</v>
       </c>
+      <c r="J291" t="n">
+        <v>45158</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -9500,6 +10375,9 @@
       <c r="I292" t="n">
         <v>0</v>
       </c>
+      <c r="J292" t="n">
+        <v>64895</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -9531,6 +10409,9 @@
       <c r="I293" t="n">
         <v>0</v>
       </c>
+      <c r="J293" t="n">
+        <v>73304</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -9562,6 +10443,9 @@
       <c r="I294" t="n">
         <v>0</v>
       </c>
+      <c r="J294" t="n">
+        <v>98793</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -9593,6 +10477,9 @@
       <c r="I295" t="n">
         <v>0</v>
       </c>
+      <c r="J295" t="n">
+        <v>116781</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -9624,6 +10511,9 @@
       <c r="I296" t="n">
         <v>0</v>
       </c>
+      <c r="J296" t="n">
+        <v>50599</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -9655,6 +10545,9 @@
       <c r="I297" t="n">
         <v>1</v>
       </c>
+      <c r="J297" t="n">
+        <v>1054965</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -9686,6 +10579,9 @@
       <c r="I298" t="n">
         <v>0</v>
       </c>
+      <c r="J298" t="n">
+        <v>15121</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -9717,6 +10613,9 @@
       <c r="I299" t="n">
         <v>0</v>
       </c>
+      <c r="J299" t="n">
+        <v>6670</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -9748,6 +10647,9 @@
       <c r="I300" t="n">
         <v>1</v>
       </c>
+      <c r="J300" t="n">
+        <v>18137</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -9779,6 +10681,9 @@
       <c r="I301" t="n">
         <v>0</v>
       </c>
+      <c r="J301" t="n">
+        <v>10084</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -9810,6 +10715,9 @@
       <c r="I302" t="n">
         <v>0</v>
       </c>
+      <c r="J302" t="n">
+        <v>28602</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -9841,6 +10749,9 @@
       <c r="I303" t="n">
         <v>0</v>
       </c>
+      <c r="J303" t="n">
+        <v>97493</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -9872,6 +10783,9 @@
       <c r="I304" t="n">
         <v>0</v>
       </c>
+      <c r="J304" t="n">
+        <v>52190</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -9903,6 +10817,9 @@
       <c r="I305" t="n">
         <v>0</v>
       </c>
+      <c r="J305" t="n">
+        <v>57365</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -9934,6 +10851,9 @@
       <c r="I306" t="n">
         <v>0</v>
       </c>
+      <c r="J306" t="n">
+        <v>70688</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -9965,6 +10885,9 @@
       <c r="I307" t="n">
         <v>0</v>
       </c>
+      <c r="J307" t="n">
+        <v>21989</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -9996,6 +10919,9 @@
       <c r="I308" t="n">
         <v>0</v>
       </c>
+      <c r="J308" t="n">
+        <v>11632</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -10027,6 +10953,9 @@
       <c r="I309" t="n">
         <v>0</v>
       </c>
+      <c r="J309" t="n">
+        <v>58031</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -10058,6 +10987,9 @@
       <c r="I310" t="n">
         <v>0</v>
       </c>
+      <c r="J310" t="n">
+        <v>35277</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -10089,6 +11021,9 @@
       <c r="I311" t="n">
         <v>0</v>
       </c>
+      <c r="J311" t="n">
+        <v>317074</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -10120,6 +11055,9 @@
       <c r="I312" t="n">
         <v>0</v>
       </c>
+      <c r="J312" t="n">
+        <v>41671</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -10151,6 +11089,9 @@
       <c r="I313" t="n">
         <v>0</v>
       </c>
+      <c r="J313" t="n">
+        <v>13128</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -10182,6 +11123,9 @@
       <c r="I314" t="n">
         <v>0</v>
       </c>
+      <c r="J314" t="n">
+        <v>142354</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -10213,6 +11157,9 @@
       <c r="I315" t="n">
         <v>0</v>
       </c>
+      <c r="J315" t="n">
+        <v>42061</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -10244,6 +11191,9 @@
       <c r="I316" t="n">
         <v>0</v>
       </c>
+      <c r="J316" t="n">
+        <v>3050869</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -10275,6 +11225,9 @@
       <c r="I317" t="n">
         <v>0</v>
       </c>
+      <c r="J317" t="n">
+        <v>52288</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -10306,6 +11259,9 @@
       <c r="I318" t="n">
         <v>0</v>
       </c>
+      <c r="J318" t="n">
+        <v>21279</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -10337,6 +11293,9 @@
       <c r="I319" t="n">
         <v>0</v>
       </c>
+      <c r="J319" t="n">
+        <v>10670</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -10368,6 +11327,9 @@
       <c r="I320" t="n">
         <v>0</v>
       </c>
+      <c r="J320" t="n">
+        <v>24895</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -10399,6 +11361,9 @@
       <c r="I321" t="n">
         <v>0</v>
       </c>
+      <c r="J321" t="n">
+        <v>94198</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -10430,6 +11395,9 @@
       <c r="I322" t="n">
         <v>0</v>
       </c>
+      <c r="J322" t="n">
+        <v>6492</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -10461,6 +11429,9 @@
       <c r="I323" t="n">
         <v>0</v>
       </c>
+      <c r="J323" t="n">
+        <v>33420</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -10492,6 +11463,9 @@
       <c r="I324" t="n">
         <v>0</v>
       </c>
+      <c r="J324" t="n">
+        <v>15098</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -10523,6 +11497,9 @@
       <c r="I325" t="n">
         <v>0</v>
       </c>
+      <c r="J325" t="n">
+        <v>119938</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -10554,6 +11531,9 @@
       <c r="I326" t="n">
         <v>0</v>
       </c>
+      <c r="J326" t="n">
+        <v>39590</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -10585,6 +11565,9 @@
       <c r="I327" t="n">
         <v>0</v>
       </c>
+      <c r="J327" t="n">
+        <v>207489</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -10616,6 +11599,9 @@
       <c r="I328" t="n">
         <v>0</v>
       </c>
+      <c r="J328" t="n">
+        <v>11783</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -10647,6 +11633,9 @@
       <c r="I329" t="n">
         <v>1</v>
       </c>
+      <c r="J329" t="n">
+        <v>122427</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -10678,6 +11667,9 @@
       <c r="I330" t="n">
         <v>0</v>
       </c>
+      <c r="J330" t="n">
+        <v>65925</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -10709,6 +11701,9 @@
       <c r="I331" t="n">
         <v>0</v>
       </c>
+      <c r="J331" t="n">
+        <v>149490</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -10740,6 +11735,9 @@
       <c r="I332" t="n">
         <v>0</v>
       </c>
+      <c r="J332" t="n">
+        <v>12247</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -10771,6 +11769,9 @@
       <c r="I333" t="n">
         <v>0</v>
       </c>
+      <c r="J333" t="n">
+        <v>56540</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -10802,6 +11803,9 @@
       <c r="I334" t="n">
         <v>0</v>
       </c>
+      <c r="J334" t="n">
+        <v>18203</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -10833,6 +11837,9 @@
       <c r="I335" t="n">
         <v>0</v>
       </c>
+      <c r="J335" t="n">
+        <v>16413</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -10864,6 +11871,9 @@
       <c r="I336" t="n">
         <v>0</v>
       </c>
+      <c r="J336" t="n">
+        <v>41789</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -10895,6 +11905,9 @@
       <c r="I337" t="n">
         <v>0</v>
       </c>
+      <c r="J337" t="n">
+        <v>1194376</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -10926,6 +11939,9 @@
       <c r="I338" t="n">
         <v>1</v>
       </c>
+      <c r="J338" t="n">
+        <v>14492</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -10957,6 +11973,9 @@
       <c r="I339" t="n">
         <v>0</v>
       </c>
+      <c r="J339" t="n">
+        <v>52620</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -10988,6 +12007,9 @@
       <c r="I340" t="n">
         <v>0</v>
       </c>
+      <c r="J340" t="n">
+        <v>46056</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -11019,6 +12041,9 @@
       <c r="I341" t="n">
         <v>0</v>
       </c>
+      <c r="J341" t="n">
+        <v>42443</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -11050,6 +12075,9 @@
       <c r="I342" t="n">
         <v>0</v>
       </c>
+      <c r="J342" t="n">
+        <v>40106</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -11081,6 +12109,9 @@
       <c r="I343" t="n">
         <v>0</v>
       </c>
+      <c r="J343" t="n">
+        <v>17089</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -11112,6 +12143,9 @@
       <c r="I344" t="n">
         <v>0</v>
       </c>
+      <c r="J344" t="n">
+        <v>35041</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -11143,6 +12177,9 @@
       <c r="I345" t="n">
         <v>0</v>
       </c>
+      <c r="J345" t="n">
+        <v>322041</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -11174,6 +12211,9 @@
       <c r="I346" t="n">
         <v>0</v>
       </c>
+      <c r="J346" t="n">
+        <v>37315</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -11205,6 +12245,9 @@
       <c r="I347" t="n">
         <v>0</v>
       </c>
+      <c r="J347" t="n">
+        <v>51267</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -11236,6 +12279,9 @@
       <c r="I348" t="n">
         <v>0</v>
       </c>
+      <c r="J348" t="n">
+        <v>115720</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -11267,6 +12313,9 @@
       <c r="I349" t="n">
         <v>1</v>
       </c>
+      <c r="J349" t="n">
+        <v>9905</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -11298,6 +12347,9 @@
       <c r="I350" t="n">
         <v>0</v>
       </c>
+      <c r="J350" t="n">
+        <v>11976</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -11329,6 +12381,9 @@
       <c r="I351" t="n">
         <v>0</v>
       </c>
+      <c r="J351" t="n">
+        <v>43229</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -11360,6 +12415,9 @@
       <c r="I352" t="n">
         <v>0</v>
       </c>
+      <c r="J352" t="n">
+        <v>48021</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -11391,6 +12449,9 @@
       <c r="I353" t="n">
         <v>0</v>
       </c>
+      <c r="J353" t="n">
+        <v>34614</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -11422,6 +12483,9 @@
       <c r="I354" t="n">
         <v>0</v>
       </c>
+      <c r="J354" t="n">
+        <v>9187</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -11453,6 +12517,9 @@
       <c r="I355" t="n">
         <v>0</v>
       </c>
+      <c r="J355" t="n">
+        <v>29700</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -11484,6 +12551,9 @@
       <c r="I356" t="n">
         <v>0</v>
       </c>
+      <c r="J356" t="n">
+        <v>232343</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -11515,6 +12585,9 @@
       <c r="I357" t="n">
         <v>0</v>
       </c>
+      <c r="J357" t="n">
+        <v>155923</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -11546,6 +12619,9 @@
       <c r="I358" t="n">
         <v>0</v>
       </c>
+      <c r="J358" t="n">
+        <v>18607</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -11577,6 +12653,9 @@
       <c r="I359" t="n">
         <v>0</v>
       </c>
+      <c r="J359" t="n">
+        <v>374401</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -11608,6 +12687,9 @@
       <c r="I360" t="n">
         <v>0</v>
       </c>
+      <c r="J360" t="n">
+        <v>105586</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -11639,6 +12721,9 @@
       <c r="I361" t="n">
         <v>0</v>
       </c>
+      <c r="J361" t="n">
+        <v>66805</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -11670,6 +12755,9 @@
       <c r="I362" t="n">
         <v>0</v>
       </c>
+      <c r="J362" t="n">
+        <v>21829</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -11701,6 +12789,9 @@
       <c r="I363" t="n">
         <v>0</v>
       </c>
+      <c r="J363" t="n">
+        <v>15064</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -11732,6 +12823,9 @@
       <c r="I364" t="n">
         <v>0</v>
       </c>
+      <c r="J364" t="n">
+        <v>123153</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -11763,6 +12857,9 @@
       <c r="I365" t="n">
         <v>0</v>
       </c>
+      <c r="J365" t="n">
+        <v>139451</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -11794,6 +12891,9 @@
       <c r="I366" t="n">
         <v>0</v>
       </c>
+      <c r="J366" t="n">
+        <v>68222</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -11825,6 +12925,9 @@
       <c r="I367" t="n">
         <v>0</v>
       </c>
+      <c r="J367" t="n">
+        <v>11576</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -11856,6 +12959,9 @@
       <c r="I368" t="n">
         <v>0</v>
       </c>
+      <c r="J368" t="n">
+        <v>8500</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -11887,6 +12993,9 @@
       <c r="I369" t="n">
         <v>0</v>
       </c>
+      <c r="J369" t="n">
+        <v>14234</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -11918,6 +13027,9 @@
       <c r="I370" t="n">
         <v>0</v>
       </c>
+      <c r="J370" t="n">
+        <v>15322</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -11949,6 +13061,9 @@
       <c r="I371" t="n">
         <v>0</v>
       </c>
+      <c r="J371" t="n">
+        <v>33128</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -11980,6 +13095,9 @@
       <c r="I372" t="n">
         <v>0</v>
       </c>
+      <c r="J372" t="n">
+        <v>19263</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -12011,6 +13129,9 @@
       <c r="I373" t="n">
         <v>0</v>
       </c>
+      <c r="J373" t="n">
+        <v>40006</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -12042,6 +13163,9 @@
       <c r="I374" t="n">
         <v>0</v>
       </c>
+      <c r="J374" t="n">
+        <v>45509</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -12073,6 +13197,9 @@
       <c r="I375" t="n">
         <v>0</v>
       </c>
+      <c r="J375" t="n">
+        <v>64079</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -12104,6 +13231,9 @@
       <c r="I376" t="n">
         <v>0</v>
       </c>
+      <c r="J376" t="n">
+        <v>21754</v>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -12135,6 +13265,9 @@
       <c r="I377" t="n">
         <v>0</v>
       </c>
+      <c r="J377" t="n">
+        <v>30090</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -12166,6 +13299,9 @@
       <c r="I378" t="n">
         <v>0</v>
       </c>
+      <c r="J378" t="n">
+        <v>51632</v>
+      </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -12197,6 +13333,9 @@
       <c r="I379" t="n">
         <v>0</v>
       </c>
+      <c r="J379" t="n">
+        <v>62440</v>
+      </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -12228,6 +13367,9 @@
       <c r="I380" t="n">
         <v>0</v>
       </c>
+      <c r="J380" t="n">
+        <v>157856</v>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -12259,6 +13401,9 @@
       <c r="I381" t="n">
         <v>0</v>
       </c>
+      <c r="J381" t="n">
+        <v>10427</v>
+      </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -12290,6 +13435,9 @@
       <c r="I382" t="n">
         <v>0</v>
       </c>
+      <c r="J382" t="n">
+        <v>29939</v>
+      </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -12321,6 +13469,9 @@
       <c r="I383" t="n">
         <v>0</v>
       </c>
+      <c r="J383" t="n">
+        <v>11582</v>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -12352,6 +13503,9 @@
       <c r="I384" t="n">
         <v>1</v>
       </c>
+      <c r="J384" t="n">
+        <v>102211</v>
+      </c>
     </row>
     <row r="385">
       <c r="A385" t="inlineStr">
@@ -12383,6 +13537,9 @@
       <c r="I385" t="n">
         <v>0</v>
       </c>
+      <c r="J385" t="n">
+        <v>17630</v>
+      </c>
     </row>
     <row r="386">
       <c r="A386" t="inlineStr">
@@ -12414,6 +13571,9 @@
       <c r="I386" t="n">
         <v>0</v>
       </c>
+      <c r="J386" t="n">
+        <v>9178</v>
+      </c>
     </row>
     <row r="387">
       <c r="A387" t="inlineStr">
@@ -12445,6 +13605,9 @@
       <c r="I387" t="n">
         <v>0</v>
       </c>
+      <c r="J387" t="n">
+        <v>24421</v>
+      </c>
     </row>
     <row r="388">
       <c r="A388" t="inlineStr">
@@ -12476,6 +13639,9 @@
       <c r="I388" t="n">
         <v>1</v>
       </c>
+      <c r="J388" t="n">
+        <v>6957</v>
+      </c>
     </row>
     <row r="389">
       <c r="A389" t="inlineStr">
@@ -12507,6 +13673,9 @@
       <c r="I389" t="n">
         <v>0</v>
       </c>
+      <c r="J389" t="n">
+        <v>28207</v>
+      </c>
     </row>
     <row r="390">
       <c r="A390" t="inlineStr">
@@ -12538,6 +13707,9 @@
       <c r="I390" t="n">
         <v>0</v>
       </c>
+      <c r="J390" t="n">
+        <v>30803</v>
+      </c>
     </row>
     <row r="391">
       <c r="A391" t="inlineStr">
@@ -12569,6 +13741,9 @@
       <c r="I391" t="n">
         <v>0</v>
       </c>
+      <c r="J391" t="n">
+        <v>19717</v>
+      </c>
     </row>
     <row r="392">
       <c r="A392" t="inlineStr">
@@ -12600,6 +13775,9 @@
       <c r="I392" t="n">
         <v>0</v>
       </c>
+      <c r="J392" t="n">
+        <v>57184</v>
+      </c>
     </row>
     <row r="393">
       <c r="A393" t="inlineStr">
@@ -12631,6 +13809,9 @@
       <c r="I393" t="n">
         <v>0</v>
       </c>
+      <c r="J393" t="n">
+        <v>47457</v>
+      </c>
     </row>
     <row r="394">
       <c r="A394" t="inlineStr">
@@ -12662,6 +13843,9 @@
       <c r="I394" t="n">
         <v>0</v>
       </c>
+      <c r="J394" t="n">
+        <v>54947</v>
+      </c>
     </row>
     <row r="395">
       <c r="A395" t="inlineStr">
@@ -12693,6 +13877,9 @@
       <c r="I395" t="n">
         <v>0</v>
       </c>
+      <c r="J395" t="n">
+        <v>119868</v>
+      </c>
     </row>
     <row r="396">
       <c r="A396" t="inlineStr">
@@ -12724,6 +13911,9 @@
       <c r="I396" t="n">
         <v>0</v>
       </c>
+      <c r="J396" t="n">
+        <v>13287</v>
+      </c>
     </row>
     <row r="397">
       <c r="A397" t="inlineStr">
@@ -12755,6 +13945,9 @@
       <c r="I397" t="n">
         <v>0</v>
       </c>
+      <c r="J397" t="n">
+        <v>27270</v>
+      </c>
     </row>
     <row r="398">
       <c r="A398" t="inlineStr">
@@ -12786,6 +13979,9 @@
       <c r="I398" t="n">
         <v>0</v>
       </c>
+      <c r="J398" t="n">
+        <v>107133</v>
+      </c>
     </row>
     <row r="399">
       <c r="A399" t="inlineStr">
@@ -12817,6 +14013,9 @@
       <c r="I399" t="n">
         <v>1</v>
       </c>
+      <c r="J399" t="n">
+        <v>115545</v>
+      </c>
     </row>
     <row r="400">
       <c r="A400" t="inlineStr">
@@ -12848,6 +14047,9 @@
       <c r="I400" t="n">
         <v>0</v>
       </c>
+      <c r="J400" t="n">
+        <v>79560</v>
+      </c>
     </row>
     <row r="401">
       <c r="A401" t="inlineStr">
@@ -12879,6 +14081,9 @@
       <c r="I401" t="n">
         <v>0</v>
       </c>
+      <c r="J401" t="n">
+        <v>13726</v>
+      </c>
     </row>
     <row r="402">
       <c r="A402" t="inlineStr">
@@ -12910,6 +14115,9 @@
       <c r="I402" t="n">
         <v>0</v>
       </c>
+      <c r="J402" t="n">
+        <v>76115</v>
+      </c>
     </row>
     <row r="403">
       <c r="A403" t="inlineStr">
@@ -12941,6 +14149,9 @@
       <c r="I403" t="n">
         <v>0</v>
       </c>
+      <c r="J403" t="n">
+        <v>14492</v>
+      </c>
     </row>
     <row r="404">
       <c r="A404" t="inlineStr">
@@ -12972,6 +14183,9 @@
       <c r="I404" t="n">
         <v>0</v>
       </c>
+      <c r="J404" t="n">
+        <v>76231</v>
+      </c>
     </row>
     <row r="405">
       <c r="A405" t="inlineStr">
@@ -13003,6 +14217,9 @@
       <c r="I405" t="n">
         <v>0</v>
       </c>
+      <c r="J405" t="n">
+        <v>73750</v>
+      </c>
     </row>
     <row r="406">
       <c r="A406" t="inlineStr">
@@ -13034,6 +14251,9 @@
       <c r="I406" t="n">
         <v>1</v>
       </c>
+      <c r="J406" t="n">
+        <v>47841</v>
+      </c>
     </row>
     <row r="407">
       <c r="A407" t="inlineStr">
@@ -13065,6 +14285,9 @@
       <c r="I407" t="n">
         <v>0</v>
       </c>
+      <c r="J407" t="n">
+        <v>132810</v>
+      </c>
     </row>
     <row r="408">
       <c r="A408" t="inlineStr">
@@ -13096,6 +14319,9 @@
       <c r="I408" t="n">
         <v>0</v>
       </c>
+      <c r="J408" t="n">
+        <v>43746</v>
+      </c>
     </row>
     <row r="409">
       <c r="A409" t="inlineStr">
@@ -13127,6 +14353,9 @@
       <c r="I409" t="n">
         <v>0</v>
       </c>
+      <c r="J409" t="n">
+        <v>22203</v>
+      </c>
     </row>
     <row r="410">
       <c r="A410" t="inlineStr">
@@ -13158,6 +14387,9 @@
       <c r="I410" t="n">
         <v>0</v>
       </c>
+      <c r="J410" t="n">
+        <v>19280</v>
+      </c>
     </row>
     <row r="411">
       <c r="A411" t="inlineStr">
@@ -13189,6 +14421,9 @@
       <c r="I411" t="n">
         <v>0</v>
       </c>
+      <c r="J411" t="n">
+        <v>22636</v>
+      </c>
     </row>
     <row r="412">
       <c r="A412" t="inlineStr">
@@ -13220,6 +14455,9 @@
       <c r="I412" t="n">
         <v>0</v>
       </c>
+      <c r="J412" t="n">
+        <v>18421</v>
+      </c>
     </row>
     <row r="413">
       <c r="A413" t="inlineStr">
@@ -13251,6 +14489,9 @@
       <c r="I413" t="n">
         <v>1</v>
       </c>
+      <c r="J413" t="n">
+        <v>45564</v>
+      </c>
     </row>
     <row r="414">
       <c r="A414" t="inlineStr">
@@ -13282,6 +14523,9 @@
       <c r="I414" t="n">
         <v>0</v>
       </c>
+      <c r="J414" t="n">
+        <v>13924</v>
+      </c>
     </row>
     <row r="415">
       <c r="A415" t="inlineStr">
@@ -13313,6 +14557,9 @@
       <c r="I415" t="n">
         <v>0</v>
       </c>
+      <c r="J415" t="n">
+        <v>16772</v>
+      </c>
     </row>
     <row r="416">
       <c r="A416" t="inlineStr">
@@ -13344,6 +14591,9 @@
       <c r="I416" t="n">
         <v>0</v>
       </c>
+      <c r="J416" t="n">
+        <v>15741</v>
+      </c>
     </row>
     <row r="417">
       <c r="A417" t="inlineStr">
@@ -13375,6 +14625,9 @@
       <c r="I417" t="n">
         <v>0</v>
       </c>
+      <c r="J417" t="n">
+        <v>119572</v>
+      </c>
     </row>
     <row r="418">
       <c r="A418" t="inlineStr">
@@ -13406,6 +14659,9 @@
       <c r="I418" t="n">
         <v>0</v>
       </c>
+      <c r="J418" t="n">
+        <v>40505</v>
+      </c>
     </row>
     <row r="419">
       <c r="A419" t="inlineStr">
@@ -13437,6 +14693,9 @@
       <c r="I419" t="n">
         <v>0</v>
       </c>
+      <c r="J419" t="n">
+        <v>121303</v>
+      </c>
     </row>
     <row r="420">
       <c r="A420" t="inlineStr">
@@ -13468,6 +14727,9 @@
       <c r="I420" t="n">
         <v>1</v>
       </c>
+      <c r="J420" t="n">
+        <v>12403</v>
+      </c>
     </row>
     <row r="421">
       <c r="A421" t="inlineStr">
@@ -13499,6 +14761,9 @@
       <c r="I421" t="n">
         <v>0</v>
       </c>
+      <c r="J421" t="n">
+        <v>63977</v>
+      </c>
     </row>
     <row r="422">
       <c r="A422" t="inlineStr">
@@ -13530,6 +14795,9 @@
       <c r="I422" t="n">
         <v>0</v>
       </c>
+      <c r="J422" t="n">
+        <v>20791</v>
+      </c>
     </row>
     <row r="423">
       <c r="A423" t="inlineStr">
@@ -13561,6 +14829,9 @@
       <c r="I423" t="n">
         <v>0</v>
       </c>
+      <c r="J423" t="n">
+        <v>10662</v>
+      </c>
     </row>
     <row r="424">
       <c r="A424" t="inlineStr">
@@ -13592,6 +14863,9 @@
       <c r="I424" t="n">
         <v>0</v>
       </c>
+      <c r="J424" t="n">
+        <v>45020</v>
+      </c>
     </row>
     <row r="425">
       <c r="A425" t="inlineStr">
@@ -13623,6 +14897,9 @@
       <c r="I425" t="n">
         <v>0</v>
       </c>
+      <c r="J425" t="n">
+        <v>16039</v>
+      </c>
     </row>
     <row r="426">
       <c r="A426" t="inlineStr">
@@ -13654,6 +14931,9 @@
       <c r="I426" t="n">
         <v>0</v>
       </c>
+      <c r="J426" t="n">
+        <v>48998</v>
+      </c>
     </row>
     <row r="427">
       <c r="A427" t="inlineStr">
@@ -13685,6 +14965,9 @@
       <c r="I427" t="n">
         <v>0</v>
       </c>
+      <c r="J427" t="n">
+        <v>10608</v>
+      </c>
     </row>
     <row r="428">
       <c r="A428" t="inlineStr">
@@ -13716,6 +14999,9 @@
       <c r="I428" t="n">
         <v>0</v>
       </c>
+      <c r="J428" t="n">
+        <v>67109</v>
+      </c>
     </row>
     <row r="429">
       <c r="A429" t="inlineStr">
@@ -13747,6 +15033,9 @@
       <c r="I429" t="n">
         <v>0</v>
       </c>
+      <c r="J429" t="n">
+        <v>110860</v>
+      </c>
     </row>
     <row r="430">
       <c r="A430" t="inlineStr">
@@ -13778,6 +15067,9 @@
       <c r="I430" t="n">
         <v>0</v>
       </c>
+      <c r="J430" t="n">
+        <v>210995</v>
+      </c>
     </row>
     <row r="431">
       <c r="A431" t="inlineStr">
@@ -13809,6 +15101,9 @@
       <c r="I431" t="n">
         <v>0</v>
       </c>
+      <c r="J431" t="n">
+        <v>191314</v>
+      </c>
     </row>
     <row r="432">
       <c r="A432" t="inlineStr">
@@ -13840,6 +15135,9 @@
       <c r="I432" t="n">
         <v>0</v>
       </c>
+      <c r="J432" t="n">
+        <v>9947</v>
+      </c>
     </row>
     <row r="433">
       <c r="A433" t="inlineStr">
@@ -13871,6 +15169,9 @@
       <c r="I433" t="n">
         <v>0</v>
       </c>
+      <c r="J433" t="n">
+        <v>19055</v>
+      </c>
     </row>
     <row r="434">
       <c r="A434" t="inlineStr">
@@ -13902,6 +15203,9 @@
       <c r="I434" t="n">
         <v>0</v>
       </c>
+      <c r="J434" t="n">
+        <v>13068</v>
+      </c>
     </row>
     <row r="435">
       <c r="A435" t="inlineStr">
@@ -13933,6 +15237,9 @@
       <c r="I435" t="n">
         <v>0</v>
       </c>
+      <c r="J435" t="n">
+        <v>23716</v>
+      </c>
     </row>
     <row r="436">
       <c r="A436" t="inlineStr">
@@ -13964,6 +15271,9 @@
       <c r="I436" t="n">
         <v>0</v>
       </c>
+      <c r="J436" t="n">
+        <v>45306</v>
+      </c>
     </row>
     <row r="437">
       <c r="A437" t="inlineStr">
@@ -13995,6 +15305,9 @@
       <c r="I437" t="n">
         <v>0</v>
       </c>
+      <c r="J437" t="n">
+        <v>21948</v>
+      </c>
     </row>
     <row r="438">
       <c r="A438" t="inlineStr">
@@ -14026,6 +15339,9 @@
       <c r="I438" t="n">
         <v>0</v>
       </c>
+      <c r="J438" t="n">
+        <v>750254</v>
+      </c>
     </row>
     <row r="439">
       <c r="A439" t="inlineStr">
@@ -14057,6 +15373,9 @@
       <c r="I439" t="n">
         <v>1</v>
       </c>
+      <c r="J439" t="n">
+        <v>15427</v>
+      </c>
     </row>
     <row r="440">
       <c r="A440" t="inlineStr">
@@ -14088,6 +15407,9 @@
       <c r="I440" t="n">
         <v>0</v>
       </c>
+      <c r="J440" t="n">
+        <v>61992</v>
+      </c>
     </row>
     <row r="441">
       <c r="A441" t="inlineStr">
@@ -14119,6 +15441,9 @@
       <c r="I441" t="n">
         <v>0</v>
       </c>
+      <c r="J441" t="n">
+        <v>27018</v>
+      </c>
     </row>
     <row r="442">
       <c r="A442" t="inlineStr">
@@ -14150,6 +15475,9 @@
       <c r="I442" t="n">
         <v>0</v>
       </c>
+      <c r="J442" t="n">
+        <v>144154</v>
+      </c>
     </row>
     <row r="443">
       <c r="A443" t="inlineStr">
@@ -14181,6 +15509,9 @@
       <c r="I443" t="n">
         <v>0</v>
       </c>
+      <c r="J443" t="n">
+        <v>16698</v>
+      </c>
     </row>
     <row r="444">
       <c r="A444" t="inlineStr">
@@ -14212,6 +15543,9 @@
       <c r="I444" t="n">
         <v>0</v>
       </c>
+      <c r="J444" t="n">
+        <v>17206</v>
+      </c>
     </row>
     <row r="445">
       <c r="A445" t="inlineStr">
@@ -14243,6 +15577,9 @@
       <c r="I445" t="n">
         <v>0</v>
       </c>
+      <c r="J445" t="n">
+        <v>13987</v>
+      </c>
     </row>
     <row r="446">
       <c r="A446" t="inlineStr">
@@ -14274,6 +15611,9 @@
       <c r="I446" t="n">
         <v>0</v>
       </c>
+      <c r="J446" t="n">
+        <v>12680</v>
+      </c>
     </row>
     <row r="447">
       <c r="A447" t="inlineStr">
@@ -14305,6 +15645,9 @@
       <c r="I447" t="n">
         <v>1</v>
       </c>
+      <c r="J447" t="n">
+        <v>10023</v>
+      </c>
     </row>
     <row r="448">
       <c r="A448" t="inlineStr">
@@ -14336,6 +15679,9 @@
       <c r="I448" t="n">
         <v>0</v>
       </c>
+      <c r="J448" t="n">
+        <v>23377</v>
+      </c>
     </row>
     <row r="449">
       <c r="A449" t="inlineStr">
@@ -14367,6 +15713,9 @@
       <c r="I449" t="n">
         <v>0</v>
       </c>
+      <c r="J449" t="n">
+        <v>486732</v>
+      </c>
     </row>
     <row r="450">
       <c r="A450" t="inlineStr">
@@ -14398,6 +15747,9 @@
       <c r="I450" t="n">
         <v>0</v>
       </c>
+      <c r="J450" t="n">
+        <v>149895</v>
+      </c>
     </row>
     <row r="451">
       <c r="A451" t="inlineStr">
@@ -14429,6 +15781,9 @@
       <c r="I451" t="n">
         <v>1</v>
       </c>
+      <c r="J451" t="n">
+        <v>114138</v>
+      </c>
     </row>
     <row r="452">
       <c r="A452" t="inlineStr">
@@ -14460,6 +15815,9 @@
       <c r="I452" t="n">
         <v>0</v>
       </c>
+      <c r="J452" t="n">
+        <v>32264</v>
+      </c>
     </row>
     <row r="453">
       <c r="A453" t="inlineStr">
@@ -14491,6 +15849,9 @@
       <c r="I453" t="n">
         <v>0</v>
       </c>
+      <c r="J453" t="n">
+        <v>63828</v>
+      </c>
     </row>
     <row r="454">
       <c r="A454" t="inlineStr">
@@ -14522,6 +15883,9 @@
       <c r="I454" t="n">
         <v>0</v>
       </c>
+      <c r="J454" t="n">
+        <v>438553</v>
+      </c>
     </row>
     <row r="455">
       <c r="A455" t="inlineStr">
@@ -14553,6 +15917,9 @@
       <c r="I455" t="n">
         <v>0</v>
       </c>
+      <c r="J455" t="n">
+        <v>6400</v>
+      </c>
     </row>
     <row r="456">
       <c r="A456" t="inlineStr">
@@ -14584,6 +15951,9 @@
       <c r="I456" t="n">
         <v>0</v>
       </c>
+      <c r="J456" t="n">
+        <v>30881</v>
+      </c>
     </row>
     <row r="457">
       <c r="A457" t="inlineStr">
@@ -14615,6 +15985,9 @@
       <c r="I457" t="n">
         <v>0</v>
       </c>
+      <c r="J457" t="n">
+        <v>44285</v>
+      </c>
     </row>
     <row r="458">
       <c r="A458" t="inlineStr">
@@ -14646,6 +16019,9 @@
       <c r="I458" t="n">
         <v>0</v>
       </c>
+      <c r="J458" t="n">
+        <v>30040</v>
+      </c>
     </row>
     <row r="459">
       <c r="A459" t="inlineStr">
@@ -14677,6 +16053,9 @@
       <c r="I459" t="n">
         <v>0</v>
       </c>
+      <c r="J459" t="n">
+        <v>35774</v>
+      </c>
     </row>
     <row r="460">
       <c r="A460" t="inlineStr">
@@ -14708,6 +16087,9 @@
       <c r="I460" t="n">
         <v>0</v>
       </c>
+      <c r="J460" t="n">
+        <v>19723</v>
+      </c>
     </row>
     <row r="461">
       <c r="A461" t="inlineStr">
@@ -14739,6 +16121,9 @@
       <c r="I461" t="n">
         <v>0</v>
       </c>
+      <c r="J461" t="n">
+        <v>107667</v>
+      </c>
     </row>
     <row r="462">
       <c r="A462" t="inlineStr">
@@ -14770,6 +16155,9 @@
       <c r="I462" t="n">
         <v>0</v>
       </c>
+      <c r="J462" t="n">
+        <v>18439</v>
+      </c>
     </row>
     <row r="463">
       <c r="A463" t="inlineStr">
@@ -14801,6 +16189,9 @@
       <c r="I463" t="n">
         <v>0</v>
       </c>
+      <c r="J463" t="n">
+        <v>14522</v>
+      </c>
     </row>
     <row r="464">
       <c r="A464" t="inlineStr">
@@ -14832,6 +16223,9 @@
       <c r="I464" t="n">
         <v>0</v>
       </c>
+      <c r="J464" t="n">
+        <v>168895</v>
+      </c>
     </row>
     <row r="465">
       <c r="A465" t="inlineStr">
@@ -14863,6 +16257,9 @@
       <c r="I465" t="n">
         <v>0</v>
       </c>
+      <c r="J465" t="n">
+        <v>24504</v>
+      </c>
     </row>
     <row r="466">
       <c r="A466" t="inlineStr">
@@ -14894,6 +16291,9 @@
       <c r="I466" t="n">
         <v>0</v>
       </c>
+      <c r="J466" t="n">
+        <v>16585</v>
+      </c>
     </row>
     <row r="467">
       <c r="A467" t="inlineStr">
@@ -14925,6 +16325,9 @@
       <c r="I467" t="n">
         <v>0</v>
       </c>
+      <c r="J467" t="n">
+        <v>18614</v>
+      </c>
     </row>
     <row r="468">
       <c r="A468" t="inlineStr">
@@ -14956,6 +16359,9 @@
       <c r="I468" t="n">
         <v>0</v>
       </c>
+      <c r="J468" t="n">
+        <v>23786</v>
+      </c>
     </row>
     <row r="469">
       <c r="A469" t="inlineStr">
@@ -14987,6 +16393,9 @@
       <c r="I469" t="n">
         <v>0</v>
       </c>
+      <c r="J469" t="n">
+        <v>18330</v>
+      </c>
     </row>
     <row r="470">
       <c r="A470" t="inlineStr">
@@ -15018,6 +16427,9 @@
       <c r="I470" t="n">
         <v>0</v>
       </c>
+      <c r="J470" t="n">
+        <v>26378</v>
+      </c>
     </row>
     <row r="471">
       <c r="A471" t="inlineStr">
@@ -15049,6 +16461,9 @@
       <c r="I471" t="n">
         <v>0</v>
       </c>
+      <c r="J471" t="n">
+        <v>47741</v>
+      </c>
     </row>
     <row r="472">
       <c r="A472" t="inlineStr">
@@ -15080,6 +16495,9 @@
       <c r="I472" t="n">
         <v>0</v>
       </c>
+      <c r="J472" t="n">
+        <v>177391</v>
+      </c>
     </row>
     <row r="473">
       <c r="A473" t="inlineStr">
@@ -15111,6 +16529,9 @@
       <c r="I473" t="n">
         <v>0</v>
       </c>
+      <c r="J473" t="n">
+        <v>6165</v>
+      </c>
     </row>
     <row r="474">
       <c r="A474" t="inlineStr">
@@ -15142,6 +16563,9 @@
       <c r="I474" t="n">
         <v>0</v>
       </c>
+      <c r="J474" t="n">
+        <v>79958</v>
+      </c>
     </row>
     <row r="475">
       <c r="A475" t="inlineStr">
@@ -15173,6 +16597,9 @@
       <c r="I475" t="n">
         <v>0</v>
       </c>
+      <c r="J475" t="n">
+        <v>42170</v>
+      </c>
     </row>
     <row r="476">
       <c r="A476" t="inlineStr">
@@ -15204,6 +16631,9 @@
       <c r="I476" t="n">
         <v>0</v>
       </c>
+      <c r="J476" t="n">
+        <v>444797</v>
+      </c>
     </row>
     <row r="477">
       <c r="A477" t="inlineStr">
@@ -15235,6 +16665,9 @@
       <c r="I477" t="n">
         <v>0</v>
       </c>
+      <c r="J477" t="n">
+        <v>20885</v>
+      </c>
     </row>
     <row r="478">
       <c r="A478" t="inlineStr">
@@ -15266,6 +16699,9 @@
       <c r="I478" t="n">
         <v>0</v>
       </c>
+      <c r="J478" t="n">
+        <v>9868</v>
+      </c>
     </row>
     <row r="479">
       <c r="A479" t="inlineStr">
@@ -15297,6 +16733,9 @@
       <c r="I479" t="n">
         <v>0</v>
       </c>
+      <c r="J479" t="n">
+        <v>25933</v>
+      </c>
     </row>
     <row r="480">
       <c r="A480" t="inlineStr">
@@ -15328,6 +16767,9 @@
       <c r="I480" t="n">
         <v>0</v>
       </c>
+      <c r="J480" t="n">
+        <v>25562</v>
+      </c>
     </row>
     <row r="481">
       <c r="A481" t="inlineStr">
@@ -15359,6 +16801,9 @@
       <c r="I481" t="n">
         <v>0</v>
       </c>
+      <c r="J481" t="n">
+        <v>22905</v>
+      </c>
     </row>
     <row r="482">
       <c r="A482" t="inlineStr">
@@ -15390,6 +16835,9 @@
       <c r="I482" t="n">
         <v>0</v>
       </c>
+      <c r="J482" t="n">
+        <v>9619</v>
+      </c>
     </row>
     <row r="483">
       <c r="A483" t="inlineStr">
@@ -15421,6 +16869,9 @@
       <c r="I483" t="n">
         <v>0</v>
       </c>
+      <c r="J483" t="n">
+        <v>32018</v>
+      </c>
     </row>
     <row r="484">
       <c r="A484" t="inlineStr">
@@ -15452,6 +16903,9 @@
       <c r="I484" t="n">
         <v>0</v>
       </c>
+      <c r="J484" t="n">
+        <v>399013</v>
+      </c>
     </row>
     <row r="485">
       <c r="A485" t="inlineStr">
@@ -15483,6 +16937,9 @@
       <c r="I485" t="n">
         <v>0</v>
       </c>
+      <c r="J485" t="n">
+        <v>7510</v>
+      </c>
     </row>
     <row r="486">
       <c r="A486" t="inlineStr">
@@ -15514,6 +16971,9 @@
       <c r="I486" t="n">
         <v>0</v>
       </c>
+      <c r="J486" t="n">
+        <v>29684</v>
+      </c>
     </row>
     <row r="487">
       <c r="A487" t="inlineStr">
@@ -15545,6 +17005,9 @@
       <c r="I487" t="n">
         <v>0</v>
       </c>
+      <c r="J487" t="n">
+        <v>36284</v>
+      </c>
     </row>
     <row r="488">
       <c r="A488" t="inlineStr">
@@ -15576,6 +17039,9 @@
       <c r="I488" t="n">
         <v>0</v>
       </c>
+      <c r="J488" t="n">
+        <v>25988</v>
+      </c>
     </row>
     <row r="489">
       <c r="A489" t="inlineStr">
@@ -15607,6 +17073,9 @@
       <c r="I489" t="n">
         <v>0</v>
       </c>
+      <c r="J489" t="n">
+        <v>13301</v>
+      </c>
     </row>
     <row r="490">
       <c r="A490" t="inlineStr">
@@ -15638,6 +17107,9 @@
       <c r="I490" t="n">
         <v>0</v>
       </c>
+      <c r="J490" t="n">
+        <v>6208</v>
+      </c>
     </row>
     <row r="491">
       <c r="A491" t="inlineStr">
@@ -15668,6 +17140,9 @@
       </c>
       <c r="I491" t="n">
         <v>0</v>
+      </c>
+      <c r="J491" t="n">
+        <v>86846</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bayesian optimization begun but gives -0.07 corrleation
</commit_message>
<xml_diff>
--- a/final_dataset.xlsx
+++ b/final_dataset.xlsx
@@ -2609,7 +2609,7 @@
         <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>0.093</v>
+        <v>0.102</v>
       </c>
       <c r="F64" t="n">
         <v>4</v>
@@ -2677,7 +2677,7 @@
         <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>1.202</v>
+        <v>1.369</v>
       </c>
       <c r="F66" t="n">
         <v>4</v>
@@ -6621,7 +6621,7 @@
         <v>0</v>
       </c>
       <c r="E182" t="n">
-        <v>0.45</v>
+        <v>0.47</v>
       </c>
       <c r="F182" t="n">
         <v>4</v>
@@ -6757,7 +6757,7 @@
         <v>0</v>
       </c>
       <c r="E186" t="n">
-        <v>2.875</v>
+        <v>2.827</v>
       </c>
       <c r="F186" t="n">
         <v>4</v>
@@ -8695,7 +8695,7 @@
         <v>0</v>
       </c>
       <c r="E243" t="n">
-        <v>0.733</v>
+        <v>0.729</v>
       </c>
       <c r="F243" t="n">
         <v>4</v>
@@ -9171,7 +9171,7 @@
         <v>0</v>
       </c>
       <c r="E257" t="n">
-        <v>0.73</v>
+        <v>0.739</v>
       </c>
       <c r="F257" t="n">
         <v>4</v>
@@ -9477,7 +9477,7 @@
         <v>0</v>
       </c>
       <c r="E266" t="n">
-        <v>0.772</v>
+        <v>0.776</v>
       </c>
       <c r="F266" t="n">
         <v>4</v>
@@ -11041,7 +11041,7 @@
         <v>1</v>
       </c>
       <c r="E312" t="n">
-        <v>12.496</v>
+        <v>12.627</v>
       </c>
       <c r="F312" t="n">
         <v>4</v>
@@ -12911,7 +12911,7 @@
         <v>0</v>
       </c>
       <c r="E367" t="n">
-        <v>0.261</v>
+        <v>0.26</v>
       </c>
       <c r="F367" t="n">
         <v>4</v>
@@ -12979,7 +12979,7 @@
         <v>0</v>
       </c>
       <c r="E369" t="n">
-        <v>0.207</v>
+        <v>0.206</v>
       </c>
       <c r="F369" t="n">
         <v>4</v>
@@ -13013,7 +13013,7 @@
         <v>0</v>
       </c>
       <c r="E370" t="n">
-        <v>2.592</v>
+        <v>2.619</v>
       </c>
       <c r="F370" t="n">
         <v>2</v>
@@ -13251,7 +13251,7 @@
         <v>0</v>
       </c>
       <c r="E377" t="n">
-        <v>0.8140000000000001</v>
+        <v>0.801</v>
       </c>
       <c r="F377" t="n">
         <v>4</v>
@@ -16719,7 +16719,7 @@
         <v>0</v>
       </c>
       <c r="E479" t="n">
-        <v>0.438</v>
+        <v>0.442</v>
       </c>
       <c r="F479" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
began cooking tobin's Q. But ACT not right
</commit_message>
<xml_diff>
--- a/final_dataset.xlsx
+++ b/final_dataset.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -2065,7 +2065,7 @@
         <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>4.527</v>
+        <v>4.505</v>
       </c>
       <c r="F48" t="n">
         <v>4</v>
@@ -2303,7 +2303,7 @@
         <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>0.114</v>
+        <v>0.116</v>
       </c>
       <c r="F55" t="n">
         <v>4</v>
@@ -2337,7 +2337,7 @@
         <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>0.126</v>
+        <v>0.127</v>
       </c>
       <c r="F56" t="n">
         <v>4</v>
@@ -2983,7 +2983,7 @@
         <v>0</v>
       </c>
       <c r="E75" t="n">
-        <v>0.027</v>
+        <v>0.03</v>
       </c>
       <c r="F75" t="n">
         <v>4</v>
@@ -3153,7 +3153,7 @@
         <v>0</v>
       </c>
       <c r="E80" t="n">
-        <v>0.207</v>
+        <v>0.211</v>
       </c>
       <c r="F80" t="n">
         <v>4</v>
@@ -6009,7 +6009,7 @@
         <v>0</v>
       </c>
       <c r="E164" t="n">
-        <v>0.7249999999999999</v>
+        <v>0.7289999999999999</v>
       </c>
       <c r="F164" t="n">
         <v>4</v>
@@ -6043,7 +6043,7 @@
         <v>0</v>
       </c>
       <c r="E165" t="n">
-        <v>0.131</v>
+        <v>0.13</v>
       </c>
       <c r="F165" t="n">
         <v>4</v>
@@ -6145,7 +6145,7 @@
         <v>0</v>
       </c>
       <c r="E168" t="n">
-        <v>1.242</v>
+        <v>1.241</v>
       </c>
       <c r="F168" t="n">
         <v>4</v>
@@ -6689,7 +6689,7 @@
         <v>0</v>
       </c>
       <c r="E184" t="n">
-        <v>0.035</v>
+        <v>0.036</v>
       </c>
       <c r="F184" t="n">
         <v>4</v>
@@ -7709,7 +7709,7 @@
         <v>1</v>
       </c>
       <c r="E214" t="n">
-        <v>9.421999999999999</v>
+        <v>9.392999999999999</v>
       </c>
       <c r="F214" t="n">
         <v>4</v>
@@ -8219,7 +8219,7 @@
         <v>0</v>
       </c>
       <c r="E229" t="n">
-        <v>0.026</v>
+        <v>0.025</v>
       </c>
       <c r="F229" t="n">
         <v>4</v>
@@ -11823,7 +11823,7 @@
         <v>0</v>
       </c>
       <c r="E335" t="n">
-        <v>0.215</v>
+        <v>0.21</v>
       </c>
       <c r="F335" t="n">
         <v>4</v>
@@ -11857,7 +11857,7 @@
         <v>0</v>
       </c>
       <c r="E336" t="n">
-        <v>0.033</v>
+        <v>0.031</v>
       </c>
       <c r="F336" t="n">
         <v>4</v>
@@ -13013,7 +13013,7 @@
         <v>0</v>
       </c>
       <c r="E370" t="n">
-        <v>2.619</v>
+        <v>2.641</v>
       </c>
       <c r="F370" t="n">
         <v>2</v>
@@ -13285,7 +13285,7 @@
         <v>0</v>
       </c>
       <c r="E378" t="n">
-        <v>0.448</v>
+        <v>0.454</v>
       </c>
       <c r="F378" t="n">
         <v>4</v>
@@ -14509,7 +14509,7 @@
         <v>0</v>
       </c>
       <c r="E414" t="n">
-        <v>0.07200000000000001</v>
+        <v>0.07100000000000001</v>
       </c>
       <c r="F414" t="n">
         <v>4</v>
@@ -15189,7 +15189,7 @@
         <v>0</v>
       </c>
       <c r="E434" t="n">
-        <v>0.225</v>
+        <v>0.226</v>
       </c>
       <c r="F434" t="n">
         <v>4</v>
@@ -15631,7 +15631,7 @@
         <v>1</v>
       </c>
       <c r="E447" t="n">
-        <v>15.632</v>
+        <v>15.883</v>
       </c>
       <c r="F447" t="n">
         <v>4</v>
@@ -17025,7 +17025,7 @@
         <v>0</v>
       </c>
       <c r="E488" t="n">
-        <v>0.05299999999999999</v>
+        <v>0.05399999999999999</v>
       </c>
       <c r="F488" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
previous sp500 companies got, not integrated
</commit_message>
<xml_diff>
--- a/final_dataset.xlsx
+++ b/final_dataset.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>